<commit_message>
updated the State Transition Matrix
</commit_message>
<xml_diff>
--- a/docs/00 dsgn doc.xlsx
+++ b/docs/00 dsgn doc.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15315" windowHeight="7995" tabRatio="765"/>
+    <workbookView xWindow="0" yWindow="48" windowWidth="15312" windowHeight="7992" tabRatio="765" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="rev control" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="122">
   <si>
     <t>Revision control</t>
   </si>
@@ -290,33 +290,6 @@
     <t>add context diagram, event list, state machine, module spec</t>
   </si>
   <si>
-    <t>COIN</t>
-  </si>
-  <si>
-    <t>IDLE</t>
-  </si>
-  <si>
-    <t>CHARGING</t>
-  </si>
-  <si>
-    <t>time + 3, display time</t>
-  </si>
-  <si>
-    <t>1MIN</t>
-  </si>
-  <si>
-    <t>2 [time &gt; 0]</t>
-  </si>
-  <si>
-    <t>1 [time = 0]</t>
-  </si>
-  <si>
-    <t>time -1, display time</t>
-  </si>
-  <si>
-    <t>time - 1, display time</t>
-  </si>
-  <si>
     <t>modify relay module, add util module</t>
   </si>
   <si>
@@ -375,13 +348,49 @@
   </si>
   <si>
     <t>change from XXX_init() into XXX_config()</t>
+  </si>
+  <si>
+    <t>The current status of X will be change to the opposite state</t>
+  </si>
+  <si>
+    <t>Corresponding LED will be ON or OFF</t>
+  </si>
+  <si>
+    <t>Touch grid X</t>
+  </si>
+  <si>
+    <t>Nothing will happen</t>
+  </si>
+  <si>
+    <t>LED will be on the previous state</t>
+  </si>
+  <si>
+    <t>Touch grid X and Y simultaneously</t>
+  </si>
+  <si>
+    <t>write mapping</t>
+  </si>
+  <si>
+    <t>check according to the XOR logic</t>
+  </si>
+  <si>
+    <t>Output as to the XOR logic</t>
+  </si>
+  <si>
+    <t>read mapping</t>
+  </si>
+  <si>
+    <t>Replace user input with the current status</t>
+  </si>
+  <si>
+    <t>Continously checking the statuses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,31 +440,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
       <sz val="14"/>
-      <color indexed="9"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,12 +480,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-        <bgColor indexed="31"/>
       </patternFill>
     </fill>
     <fill>
@@ -512,12 +520,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor indexed="34"/>
+        <fgColor rgb="FF800080"/>
+        <bgColor rgb="FF800080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -612,35 +632,7 @@
       <top style="thin">
         <color indexed="63"/>
       </top>
-      <bottom style="thin">
-        <color indexed="63"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="63"/>
-      </left>
-      <right style="thin">
-        <color indexed="63"/>
-      </right>
-      <top style="thin">
-        <color indexed="63"/>
-      </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="63"/>
-      </left>
-      <right style="thin">
-        <color indexed="63"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="63"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -699,41 +691,165 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="1">
+    <border>
       <left style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </left>
       <right style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </right>
       <top style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF333333"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF333333"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF333333"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF333333"/>
       </top>
       <bottom/>
-      <diagonal style="thin">
-        <color indexed="63"/>
-      </diagonal>
+      <diagonal/>
     </border>
-    <border diagonalDown="1">
+    <border>
       <left style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </left>
       <right style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </bottom>
-      <diagonal style="thin">
-        <color indexed="63"/>
-      </diagonal>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF333333"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF333333"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF333333"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF333333"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF333333"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF333333"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF333333"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF333333"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF333333"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF333333"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF333333"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF333333"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -762,7 +878,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -789,34 +905,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -824,38 +940,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -875,16 +967,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -893,12 +979,83 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -4642,6 +4799,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -4676,6 +4834,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4851,40 +5010,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="85.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="5.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="85.6640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="26.1" customHeight="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="26.1" customHeight="1">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="24.9" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -4927,7 +5086,7 @@
         <v>0.2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E5" s="5"/>
     </row>
@@ -4942,7 +5101,7 @@
         <v>0.3</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E6" s="5"/>
     </row>
@@ -5059,38 +5218,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="9" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="9" customWidth="1"/>
+    <col min="3" max="4" width="25.6640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:5" ht="24.6">
+      <c r="A1" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-    </row>
-    <row r="2" spans="1:5" ht="25.5">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-    </row>
-    <row r="3" spans="1:5" ht="24.95" customHeight="1">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+    </row>
+    <row r="2" spans="1:5" ht="24.6">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+    </row>
+    <row r="3" spans="1:5" ht="24.9" customHeight="1">
       <c r="A3" s="21" t="s">
         <v>10</v>
       </c>
@@ -5124,7 +5283,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="5" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
       <c r="A5" s="28" t="s">
         <v>26</v>
       </c>
@@ -5141,7 +5300,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="6" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
       <c r="A6" s="28" t="s">
         <v>30</v>
       </c>
@@ -5158,28 +5317,28 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="7" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
       <c r="A7" s="28"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
     </row>
-    <row r="8" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="8" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
       <c r="A8" s="28"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
     </row>
-    <row r="9" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="9" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
       <c r="A9" s="28"/>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="10" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
       <c r="A10" s="29"/>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
@@ -5197,29 +5356,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="110.7109375" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="15.6640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="110.6640625" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="11" customFormat="1" ht="25.5">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:2" s="11" customFormat="1" ht="24.6">
+      <c r="A1" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="49"/>
-    </row>
-    <row r="2" spans="1:2" s="11" customFormat="1" ht="25.5">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
+      <c r="B1" s="41"/>
+    </row>
+    <row r="2" spans="1:2" s="11" customFormat="1" ht="24.6">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
     </row>
     <row r="3" spans="1:2" s="14" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="12" t="s">
@@ -5383,189 +5542,221 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="9" customWidth="1"/>
-    <col min="3" max="5" width="30.7109375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="9" customWidth="1"/>
+    <col min="3" max="5" width="30.6640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="33" customFormat="1" ht="25.5">
-      <c r="B1" s="52" t="s">
+    <row r="1" spans="1:5" s="33" customFormat="1" ht="24.6">
+      <c r="A1" s="47"/>
+      <c r="B1" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-    </row>
-    <row r="2" spans="1:5" s="33" customFormat="1" ht="25.5">
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-    </row>
-    <row r="3" spans="1:5" ht="24.95" customHeight="1">
-      <c r="A3" s="34"/>
-      <c r="B3" s="53" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+    </row>
+    <row r="2" spans="1:5" s="33" customFormat="1" ht="24.6">
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+    </row>
+    <row r="3" spans="1:5" ht="24.9" customHeight="1">
+      <c r="A3" s="50"/>
+      <c r="B3" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="36"/>
-    </row>
-    <row r="4" spans="1:5" ht="24.95" customHeight="1">
-      <c r="A4" s="34"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="37">
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="53"/>
+    </row>
+    <row r="4" spans="1:5" ht="24.9" customHeight="1">
+      <c r="A4" s="50"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="54">
         <v>1</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="54">
         <v>2</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="54">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="40">
+      <c r="B5" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="59">
+        <v>1</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="57" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+    </row>
+    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="55"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="67">
         <v>2</v>
       </c>
-      <c r="D5" s="40">
-        <v>2</v>
-      </c>
-      <c r="E5" s="40"/>
-    </row>
-    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="41"/>
-    </row>
-    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="14" t="s">
+      <c r="D7" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="70" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="55"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="71"/>
+      <c r="E8" s="72"/>
+    </row>
+    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="40"/>
-    </row>
-    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="41"/>
-    </row>
-    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="14" t="s">
+      <c r="B9" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="59">
+        <v>1</v>
+      </c>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+    </row>
+    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="55"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="40"/>
-    </row>
-    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="41"/>
-    </row>
-    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="14" t="s">
+      <c r="B11" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="59">
+        <v>1</v>
+      </c>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+    </row>
+    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="55"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-    </row>
-    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-    </row>
-    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="14" t="s">
+      <c r="B13" s="65"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+    </row>
+    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="55"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+    </row>
+    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-    </row>
-    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-    </row>
-    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="14" t="s">
+      <c r="B15" s="65"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+    </row>
+    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="55"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-    </row>
-    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="1"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="55"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -5573,334 +5764,334 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:5" ht="24.6">
+      <c r="A1" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-    </row>
-    <row r="2" spans="1:5" s="33" customFormat="1" ht="25.5"/>
-    <row r="3" spans="1:5" ht="19.899999999999999" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+    </row>
+    <row r="2" spans="1:5" s="33" customFormat="1" ht="24.6"/>
+    <row r="3" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A3" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="34" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="39" t="s">
+      <c r="B4" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="39" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1">
-      <c r="A6" s="55"/>
-      <c r="B6" s="39" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1">
-      <c r="A7" s="56"/>
-      <c r="B7" s="39" t="s">
+      <c r="A7" s="46"/>
+      <c r="B7" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="39" t="s">
+      <c r="B8" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1">
-      <c r="A9" s="55"/>
-      <c r="B9" s="39" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1">
-      <c r="A10" s="56"/>
-      <c r="B10" s="39" t="s">
+      <c r="A10" s="46"/>
+      <c r="B10" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="39" t="s">
+      <c r="B11" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" customHeight="1">
-      <c r="A12" s="55"/>
-      <c r="B12" s="39" t="s">
+      <c r="A12" s="45"/>
+      <c r="B12" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1">
-      <c r="A13" s="55"/>
-      <c r="B13" s="39" t="s">
+      <c r="A13" s="45"/>
+      <c r="B13" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1">
-      <c r="A14" s="56"/>
-      <c r="B14" s="39" t="s">
+      <c r="A14" s="46"/>
+      <c r="B14" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="35" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="D15" s="39" t="s">
+      <c r="B15" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1">
-      <c r="A16" s="55"/>
-      <c r="B16" s="39" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1">
+      <c r="A17" s="46"/>
+      <c r="B17" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" customHeight="1">
+      <c r="A18" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" customHeight="1">
+      <c r="A19" s="45"/>
+      <c r="B19" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="39" t="s">
+      <c r="D19" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="35" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" s="56"/>
-      <c r="B17" s="39" t="s">
+    <row r="20" spans="1:5" ht="30" customHeight="1">
+      <c r="A20" s="46"/>
+      <c r="B20" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" customHeight="1">
-      <c r="A18" s="54" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" customHeight="1">
-      <c r="A19" s="55"/>
-      <c r="B19" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" customHeight="1">
-      <c r="A20" s="56"/>
-      <c r="B20" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="21" spans="1:5" ht="30" customHeight="1">
-      <c r="A21" s="42"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1">
-      <c r="A22" s="39"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1">
-      <c r="A23" s="39"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
updated the event list
</commit_message>
<xml_diff>
--- a/docs/00 dsgn doc.xlsx
+++ b/docs/00 dsgn doc.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\AppData\Local\Temp\docs.svn000.tmp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="15312" windowHeight="7992" tabRatio="765" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15315" windowHeight="7995" tabRatio="765" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rev control" sheetId="1" r:id="rId1"/>
@@ -849,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -905,34 +910,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -948,6 +932,40 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -967,9 +985,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -979,72 +1026,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,6 +1062,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -4767,7 +4778,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4802,7 +4813,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5017,33 +5028,33 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="85.6640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="9"/>
+    <col min="1" max="1" width="5.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="85.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="26.1" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="26.1" customHeight="1">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="24.9" customHeight="1">
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="24.95" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -5064,7 +5075,7 @@
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="21">
         <v>41939</v>
       </c>
       <c r="C4" s="4">
@@ -5079,7 +5090,7 @@
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="21">
         <v>41947</v>
       </c>
       <c r="C5" s="4">
@@ -5094,7 +5105,7 @@
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="21">
         <v>41947</v>
       </c>
       <c r="C6" s="4">
@@ -5221,129 +5232,129 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="9" customWidth="1"/>
-    <col min="3" max="4" width="25.6640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="9" customWidth="1"/>
+    <col min="3" max="4" width="25.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24.6">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:5" ht="25.5">
+      <c r="A1" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-    </row>
-    <row r="2" spans="1:5" ht="24.6">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-    </row>
-    <row r="3" spans="1:5" ht="24.9" customHeight="1">
-      <c r="A3" s="21" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+    </row>
+    <row r="2" spans="1:5" ht="25.5">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+    </row>
+    <row r="3" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A3" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="70" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="20" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="71" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A5" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="72" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A6" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="72" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-    </row>
-    <row r="8" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-    </row>
-    <row r="9" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-    </row>
-    <row r="10" spans="1:5" s="20" customFormat="1" ht="39.9" customHeight="1">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
+    <row r="7" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A7" s="72"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+    </row>
+    <row r="8" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="1:5" s="20" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5363,22 +5374,22 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="110.6640625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="10"/>
+    <col min="1" max="1" width="15.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="110.7109375" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="11" customFormat="1" ht="24.6">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:2" s="11" customFormat="1" ht="25.5">
+      <c r="A1" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="41"/>
-    </row>
-    <row r="2" spans="1:2" s="11" customFormat="1" ht="24.6">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
+      <c r="B1" s="46"/>
+    </row>
+    <row r="2" spans="1:2" s="11" customFormat="1" ht="25.5">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
     </row>
     <row r="3" spans="1:2" s="14" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="12" t="s">
@@ -5398,13 +5409,13 @@
     </row>
     <row r="5" spans="1:2" s="14" customFormat="1" ht="200.1" customHeight="1">
       <c r="A5" s="16"/>
-      <c r="B5" s="31"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" s="14" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="25"/>
     </row>
     <row r="7" spans="1:2" s="14" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="12" t="s">
@@ -5545,63 +5556,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="9" customWidth="1"/>
-    <col min="3" max="5" width="30.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="9" customWidth="1"/>
+    <col min="3" max="5" width="30.7109375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="33" customFormat="1" ht="24.6">
-      <c r="A1" s="47"/>
-      <c r="B1" s="48" t="s">
+    <row r="1" spans="1:5" s="26" customFormat="1" ht="25.5">
+      <c r="A1" s="30"/>
+      <c r="B1" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-    </row>
-    <row r="2" spans="1:5" s="33" customFormat="1" ht="24.6">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-    </row>
-    <row r="3" spans="1:5" ht="24.9" customHeight="1">
-      <c r="A3" s="50"/>
-      <c r="B3" s="51" t="s">
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+    </row>
+    <row r="2" spans="1:5" s="26" customFormat="1" ht="25.5">
+      <c r="A2" s="30"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+    </row>
+    <row r="3" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A3" s="31"/>
+      <c r="B3" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="53"/>
-    </row>
-    <row r="4" spans="1:5" ht="24.9" customHeight="1">
-      <c r="A4" s="50"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="54">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A4" s="31"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="34">
         <v>1</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="34">
         <v>2</v>
       </c>
-      <c r="E4" s="54">
+      <c r="E4" s="34">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="59">
+      <c r="C5" s="38">
         <v>1</v>
       </c>
       <c r="D5" s="57" t="s">
@@ -5612,135 +5623,135 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="55"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="60" t="s">
+      <c r="A6" s="35"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="55"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="67">
+      <c r="A7" s="35"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="40">
         <v>2</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="70" t="s">
+      <c r="E7" s="60" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="55"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="67" t="s">
+      <c r="A8" s="35"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="71"/>
-      <c r="E8" s="72"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="61"/>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="59">
+      <c r="C9" s="38">
         <v>1</v>
       </c>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="55"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="60" t="s">
+      <c r="A10" s="35"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="58" t="s">
+      <c r="D10" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="37" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="59">
+      <c r="C11" s="38">
         <v>1</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="55"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="60" t="s">
+      <c r="A12" s="35"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="37" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
     </row>
     <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="55"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
     </row>
     <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="65"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="55"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="55"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -5771,327 +5782,327 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24.6">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:5" ht="25.5">
+      <c r="A1" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-    </row>
-    <row r="2" spans="1:5" s="33" customFormat="1" ht="24.6"/>
-    <row r="3" spans="1:5" ht="19.95" customHeight="1">
-      <c r="A3" s="34" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+    </row>
+    <row r="2" spans="1:5" s="26" customFormat="1" ht="25.5"/>
+    <row r="3" spans="1:5" ht="19.899999999999999" customHeight="1">
+      <c r="A3" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="27" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="35" t="s">
+      <c r="A5" s="63"/>
+      <c r="B5" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="35" t="s">
+      <c r="A6" s="63"/>
+      <c r="B6" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1">
-      <c r="A7" s="46"/>
-      <c r="B7" s="35" t="s">
+      <c r="A7" s="64"/>
+      <c r="B7" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1">
-      <c r="A9" s="45"/>
-      <c r="B9" s="35" t="s">
+      <c r="A9" s="63"/>
+      <c r="B9" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1">
-      <c r="A10" s="46"/>
-      <c r="B10" s="35" t="s">
+      <c r="A10" s="64"/>
+      <c r="B10" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" customHeight="1">
-      <c r="A12" s="45"/>
-      <c r="B12" s="35" t="s">
+      <c r="A12" s="63"/>
+      <c r="B12" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1">
-      <c r="A13" s="45"/>
-      <c r="B13" s="35" t="s">
+      <c r="A13" s="63"/>
+      <c r="B13" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1">
-      <c r="A14" s="46"/>
-      <c r="B14" s="35" t="s">
+      <c r="A14" s="64"/>
+      <c r="B14" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="28" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1">
-      <c r="A16" s="45"/>
-      <c r="B16" s="35" t="s">
+      <c r="A16" s="63"/>
+      <c r="B16" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" s="46"/>
-      <c r="B17" s="35" t="s">
+      <c r="A17" s="64"/>
+      <c r="B17" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1">
-      <c r="A19" s="45"/>
-      <c r="B19" s="35" t="s">
+      <c r="A19" s="63"/>
+      <c r="B19" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" customHeight="1">
-      <c r="A20" s="46"/>
-      <c r="B20" s="35" t="s">
+      <c r="A20" s="64"/>
+      <c r="B20" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="28" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" customHeight="1">
-      <c r="A21" s="36"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Modify the Module Specification of design document
</commit_message>
<xml_diff>
--- a/docs/00 dsgn doc.xlsx
+++ b/docs/00 dsgn doc.xlsx
@@ -1008,13 +1008,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1053,6 +1046,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5383,14 +5383,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="11" customFormat="1" ht="25.5">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" s="11" customFormat="1" ht="25.5">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
     </row>
     <row r="3" spans="1:2" s="14" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="12" t="s">
@@ -5570,23 +5570,23 @@
   <sheetData>
     <row r="1" spans="1:5" s="26" customFormat="1" ht="25.5">
       <c r="A1" s="27"/>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:5" s="26" customFormat="1" ht="25.5">
       <c r="A2" s="27"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="1:5" ht="24.95" customHeight="1">
       <c r="A3" s="28"/>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="63" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="29"/>
@@ -5595,7 +5595,7 @@
     </row>
     <row r="4" spans="1:5" ht="24.95" customHeight="1">
       <c r="A4" s="28"/>
-      <c r="B4" s="65"/>
+      <c r="B4" s="62"/>
       <c r="C4" s="31">
         <v>1</v>
       </c>
@@ -5610,55 +5610,55 @@
       <c r="A5" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="65" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="35">
         <v>1</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="66" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="32"/>
-      <c r="B6" s="63"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="32"/>
-      <c r="B7" s="63"/>
+      <c r="B7" s="60"/>
       <c r="C7" s="37">
         <v>2</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="E7" s="72" t="s">
+      <c r="E7" s="69" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="32"/>
-      <c r="B8" s="63"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="71"/>
-      <c r="E8" s="73"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="70"/>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="64" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="35">
@@ -5669,7 +5669,7 @@
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="32"/>
-      <c r="B10" s="63"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="36" t="s">
         <v>98</v>
       </c>
@@ -5684,7 +5684,7 @@
       <c r="A11" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="59" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="35">
@@ -5695,7 +5695,7 @@
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="32"/>
-      <c r="B12" s="63"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="36" t="s">
         <v>101</v>
       </c>
@@ -5710,14 +5710,14 @@
       <c r="A13" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="60"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="35"/>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
     </row>
     <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="32"/>
-      <c r="B14" s="63"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="36"/>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
@@ -5726,14 +5726,14 @@
       <c r="A15" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="60"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="35"/>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="32"/>
-      <c r="B16" s="63"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
@@ -5742,14 +5742,14 @@
       <c r="A17" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="60"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="35"/>
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="32"/>
-      <c r="B18" s="61"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
@@ -5780,25 +5780,26 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.5">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="1:5" ht="25.5">
       <c r="A2" s="48"/>
@@ -5825,7 +5826,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.5">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="73" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="47" t="s">
@@ -5842,7 +5843,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="56"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="47" t="s">
         <v>59</v>
       </c>
@@ -5857,7 +5858,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="56"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="47" t="s">
         <v>60</v>
       </c>
@@ -5872,7 +5873,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.5">
-      <c r="A7" s="56"/>
+      <c r="A7" s="72"/>
       <c r="B7" s="47" t="s">
         <v>61</v>
       </c>
@@ -5887,7 +5888,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.5">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="73" t="s">
         <v>68</v>
       </c>
       <c r="B8" s="47" t="s">
@@ -5904,7 +5905,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.5">
-      <c r="A9" s="56"/>
+      <c r="A9" s="72"/>
       <c r="B9" s="47" t="s">
         <v>69</v>
       </c>
@@ -5919,7 +5920,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="56"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="47" t="s">
         <v>70</v>
       </c>
@@ -5934,7 +5935,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="73" t="s">
         <v>75</v>
       </c>
       <c r="B11" s="47" t="s">
@@ -5951,7 +5952,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.5">
-      <c r="A12" s="56"/>
+      <c r="A12" s="72"/>
       <c r="B12" s="47" t="s">
         <v>77</v>
       </c>
@@ -5966,7 +5967,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.5">
-      <c r="A13" s="56"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="47" t="s">
         <v>76</v>
       </c>
@@ -5981,7 +5982,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5">
-      <c r="A14" s="56"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="47" t="s">
         <v>78</v>
       </c>
@@ -5994,7 +5995,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.5">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="73" t="s">
         <v>86</v>
       </c>
       <c r="B15" s="47" t="s">
@@ -6011,7 +6012,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="28.5">
-      <c r="A16" s="56"/>
+      <c r="A16" s="72"/>
       <c r="B16" s="47" t="s">
         <v>109</v>
       </c>

</xml_diff>

<commit_message>
testing the relay.c file and debugging the Util.c file.
</commit_message>
<xml_diff>
--- a/docs/00 dsgn doc.xlsx
+++ b/docs/00 dsgn doc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RUSHA_~1\AppData\Local\Temp\docs.svn000.tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\ait-embsys-doorlocksystem\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5026,7 +5026,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -5118,7 +5118,9 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="4"/>
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
       <c r="B7" s="5"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
@@ -5557,7 +5559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7:E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>